<commit_message>
Added ExcelUtils.java - getSheetIntoTwoDimArray
</commit_message>
<xml_diff>
--- a/test_data/orange_data.xlsx
+++ b/test_data/orange_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JiDi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mine\Company\MicroFocus3\HybridFramework\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -371,7 +371,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Common data provider for valid and invalid login test
</commit_message>
<xml_diff>
--- a/test_data/orange_data.xlsx
+++ b/test_data/orange_data.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="4584" windowHeight="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="4584" windowHeight="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="invalidLoginTest" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="validLoginTest" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
+    <sheet name="addEmployeeTest" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>User Name</t>
   </si>
@@ -47,10 +48,61 @@
     <t>Invalid credentials</t>
   </si>
   <si>
-    <t>kim</t>
-  </si>
-  <si>
-    <t>kim123</t>
+    <t>bala</t>
+  </si>
+  <si>
+    <t>bala123</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Expected Header</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Expected Profile Name</t>
+  </si>
+  <si>
+    <t>Bala</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Dina</t>
+  </si>
+  <si>
+    <t>Bala Dina</t>
+  </si>
+  <si>
+    <t>Saul</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>goodman</t>
+  </si>
+  <si>
+    <t>Saul goodman</t>
   </si>
 </sst>
 </file>
@@ -370,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -394,10 +446,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -405,10 +457,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -421,12 +473,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -453,4 +530,87 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>